<commit_message>
added 5 6 7
</commit_message>
<xml_diff>
--- a/Docenza_Conti_UFS01 - Sistemi Operativi e gestione della concorrenza.xlsx
+++ b/Docenza_Conti_UFS01 - Sistemi Operativi e gestione della concorrenza.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/BigSur_110/Users/ingconti/Documents/GIT-BigSur/its_rizzoli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F75D9E7-679C-DA44-90C2-DC26030EF63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324577AC-5B4E-E745-B224-25BCEA0049EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
   <si>
     <t>Data</t>
   </si>
@@ -119,6 +119,36 @@
   </si>
   <si>
     <t>FAD in ITS 3</t>
+  </si>
+  <si>
+    <t>7. Gestione del File System</t>
+  </si>
+  <si>
+    <t>8. Gestione della Memoria e memoria virtuale</t>
+  </si>
+  <si>
+    <t>9. Processi e Risorse, Calcolo Parallelo e Distribuito</t>
+  </si>
+  <si>
+    <t>10. La concorrenza: Il modello a processi; Processi sequenziali e paralleli, I Thread</t>
+  </si>
+  <si>
+    <t>11. Elaborazione sequenziale e concorrente, La Concorrenza tra processi</t>
+  </si>
+  <si>
+    <t>12. Scheduling della CPU e Algoritmi di scheduling: sincronizzazione e comunicazione tra processi</t>
+  </si>
+  <si>
+    <t>13. Sezione critica e mutua esclusione</t>
+  </si>
+  <si>
+    <t>14. I semafori, produttori/consumatori, lettori/scrittori, deadlock, monitor e scambio di messaggi</t>
+  </si>
+  <si>
+    <t>15. Comandi fondamentali di Linux e bash scripting</t>
+  </si>
+  <si>
+    <t>16. Comandi fondamentali di dos/PowerShell scripting</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1030,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:H9"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1018,7 +1048,7 @@
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="5">
         <v>44496</v>
       </c>
@@ -1070,7 +1100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
         <v>44503</v>
       </c>
@@ -1096,7 +1126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="6"/>
@@ -1106,7 +1136,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>44518</v>
       </c>
@@ -1132,7 +1162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>44524</v>
       </c>
@@ -1158,7 +1188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>44525</v>
       </c>
@@ -1184,7 +1214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>44529</v>
       </c>
@@ -1210,7 +1240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>44531</v>
       </c>
@@ -1235,8 +1265,11 @@
       <c r="H9" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>44532</v>
       </c>
@@ -1261,8 +1294,11 @@
       <c r="H10" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="5">
         <v>44540</v>
       </c>
@@ -1287,8 +1323,11 @@
       <c r="H11" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <v>44543</v>
       </c>
@@ -1313,8 +1352,11 @@
       <c r="H12" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
         <v>44545</v>
       </c>
@@ -1339,8 +1381,11 @@
       <c r="H13" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>44573</v>
       </c>
@@ -1365,8 +1410,11 @@
       <c r="H14" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I14" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
         <v>44575</v>
       </c>
@@ -1391,8 +1439,11 @@
       <c r="H15" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>44578</v>
       </c>
@@ -1417,8 +1468,11 @@
       <c r="H16" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="5">
         <v>44578</v>
       </c>
@@ -1443,8 +1497,11 @@
       <c r="H17" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="I17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="5">
         <v>44586</v>
       </c>
@@ -1468,6 +1525,9 @@
       </c>
       <c r="H18" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>